<commit_message>
get word counts and model society class with them
</commit_message>
<xml_diff>
--- a/lexicons/enh_conflict_lexicon.xlsx
+++ b/lexicons/enh_conflict_lexicon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmackenzie/Documents/Github/peace-speech-project/lexicons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattb\Documents\GitHub\peace-speech-project\lexicons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18FCBFA-0222-9D43-BE55-C1D28A33282B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9094850B-73EF-429F-8C2A-14B3F7063C1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enh_conflict_lexicon" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="751">
   <si>
     <t>Term</t>
   </si>
@@ -370,9 +370,6 @@
   </si>
   <si>
     <t>caste system</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>challenge</t>
@@ -2546,15 +2543,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B995"/>
+  <dimension ref="A1:A995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="14.5" customWidth="1"/>
+    <col min="1" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3117,3454 +3114,3445 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B115" s="1" t="s">
+    </row>
+    <row r="116" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
+    <row r="122" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
+    <row r="123" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
+    <row r="124" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
+    <row r="125" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
+    <row r="126" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
+    <row r="127" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
+    <row r="128" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="176" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="177" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="180" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="183" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="184" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="185" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="186" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="187" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="189" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="190" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="193" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="194" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="195" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="196" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="197" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="198" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="201" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="203" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="204" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="205" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="206" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="207" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="208" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="209" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="210" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="211" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="212" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="213" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="214" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="215" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="216" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="217" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="218" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="219" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="220" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="221" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="222" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="223" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="224" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="225" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="226" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="227" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="228" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="229" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="230" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="231" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="232" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="233" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="234" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="235" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="236" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="237" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="238" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="239" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="240" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="241" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="242" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="243" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="244" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="245" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="246" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="247" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="248" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="249" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="250" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="251" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="252" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="253" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="254" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="255" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="256" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="257" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="258" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="259" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="260" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="261" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="262" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="263" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="264" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="265" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="266" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="267" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="268" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="269" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="270" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="271" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="272" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="273" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="274" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="275" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="276" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="277" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="278" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="279" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="280" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="281" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="282" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="283" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="284" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="285" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="286" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="287" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="288" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="289" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="290" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="291" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="292" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="293" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="294" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="295" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="296" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="297" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="298" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="299" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="300" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="301" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="302" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="303" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="304" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="305" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="306" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="307" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="308" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="309" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="310" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="311" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="312" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="313" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="314" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="315" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="316" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="317" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="318" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="319" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="320" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="321" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="322" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="323" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="324" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="325" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="326" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="327" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="328" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="329" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="330" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="331" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="332" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="333" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="334" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="335" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="336" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="337" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="338" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="339" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="340" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="341" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="342" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="343" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="344" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="345" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="346" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="347" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="348" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="349" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="350" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="351" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="352" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="353" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A353" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="354" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="355" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="356" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="357" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="358" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="359" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="360" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="361" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="362" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="363" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A363" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="364" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="365" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A365" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="366" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="367" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A367" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="368" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="369" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A369" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="370" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="371" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A371" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="372" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A372" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="373" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A373" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="374" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="375" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A375" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="376" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="377" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A377" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="378" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="379" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="380" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A380" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="381" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A381" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="382" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A382" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="383" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A383" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="384" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A384" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="385" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A385" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="386" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A386" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="387" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A387" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="388" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A388" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="389" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A389" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="390" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A390" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="391" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A391" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="392" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A392" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="393" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A393" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="394" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="395" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A395" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="396" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="397" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A397" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="398" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="399" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A399" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="400" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A400" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="401" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A401" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="402" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A402" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="403" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A403" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="404" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A404" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="405" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A405" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="406" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="407" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A407" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="408" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="409" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="410" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="411" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A411" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="412" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="413" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A413" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="414" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A414" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="415" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A415" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="416" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A416" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="417" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A417" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="418" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A418" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="419" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A419" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="420" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A420" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="421" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A421" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="422" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A422" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="423" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A423" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="424" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A424" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="425" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A425" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="426" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A426" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="427" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A427" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="428" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A428" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="429" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A429" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="430" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A430" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="431" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A431" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="432" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A432" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="433" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A433" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="434" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A434" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="435" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A435" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="436" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A436" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="437" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A437" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="438" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A438" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="439" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A439" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="440" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A440" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="441" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A441" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="442" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A442" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="443" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A443" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="444" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A444" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="445" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A445" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="446" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A446" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="447" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A447" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="448" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A448" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="449" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A449" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="450" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="451" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A451" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="452" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="453" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A453" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="454" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A454" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="455" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A455" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="456" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A456" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="457" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A457" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="458" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A458" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="459" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A459" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="460" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A460" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="461" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A461" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="462" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A462" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="463" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A463" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="464" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A464" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="465" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A465" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="466" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A466" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="467" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A467" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="468" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A468" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="469" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A469" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="470" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A470" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="471" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A471" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="472" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A472" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="473" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A473" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="474" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A474" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="475" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A475" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="476" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A476" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="477" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A477" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="478" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A478" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="479" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A479" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="480" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A480" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="481" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A481" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="482" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A482" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="483" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A483" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="484" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A484" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="485" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A485" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="486" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A486" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="487" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A487" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="488" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A488" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="489" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A489" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="490" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A490" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="491" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A491" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="492" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A492" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="493" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A493" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="494" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A494" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="495" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A495" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="496" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A496" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A497" s="1" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="497" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A497" s="1" t="s">
+    <row r="498" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A498" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="498" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A498" s="1" t="s">
+    <row r="499" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A499" s="1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="499" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A499" s="1" t="s">
+    <row r="500" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A500" s="1" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="500" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A500" s="1" t="s">
+    <row r="501" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A501" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="501" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A501" s="1" t="s">
+    <row r="502" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A502" s="1" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="502" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A502" s="1" t="s">
+    <row r="503" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A503" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="503" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A503" s="1" t="s">
+    <row r="504" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A504" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="504" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A504" s="1" t="s">
+    <row r="505" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A505" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="B504" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="505" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A505" s="1" t="s">
+    </row>
+    <row r="506" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A506" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="B505" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="506" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A506" s="1" t="s">
+    </row>
+    <row r="507" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A507" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="507" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A507" s="1" t="s">
+    <row r="508" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A508" s="1" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="508" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A508" s="1" t="s">
+    <row r="509" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A509" s="1" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="509" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A509" s="1" t="s">
+    <row r="510" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A510" s="1" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="510" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A510" s="1" t="s">
+    <row r="511" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A511" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="511" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A511" s="1" t="s">
+    <row r="512" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A512" s="1" t="s">
         <v>511</v>
-      </c>
-    </row>
-    <row r="512" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A512" s="1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="513" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A513" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="514" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A514" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="515" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A515" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="516" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A516" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="517" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A517" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="518" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A518" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="519" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A519" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="520" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A520" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="521" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A521" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="522" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A522" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="523" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A523" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="524" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A524" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="525" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A525" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="526" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A526" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="527" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A527" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="528" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A528" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="529" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A529" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="530" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A530" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="531" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A531" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="532" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A532" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="533" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A533" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="534" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A534" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="535" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A535" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="536" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A536" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="537" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A537" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="538" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A538" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="539" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A539" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="540" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A540" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="541" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A541" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="542" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="543" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A543" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="544" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A544" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="545" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A545" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="546" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A546" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="547" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A547" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="548" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A548" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="549" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A549" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="550" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A550" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="551" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A551" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="552" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A552" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="553" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A553" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="554" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A554" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="555" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A555" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="556" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A556" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="557" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A557" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="558" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A558" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="559" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A559" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="560" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A560" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="561" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A561" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="562" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A562" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="563" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A563" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="564" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A564" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="565" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A565" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="566" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A566" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="567" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A567" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="568" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A568" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="569" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A569" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="570" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A570" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="571" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A571" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="572" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A572" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="573" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A573" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="574" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A574" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="575" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A575" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="576" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A576" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="577" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A577" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="578" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A578" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="579" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A579" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="580" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A580" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="581" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A581" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="582" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A582" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="583" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A583" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="584" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A584" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="585" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A585" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="586" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A586" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="587" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A587" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="588" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A588" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="589" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A589" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="590" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A590" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="591" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A591" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="592" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A592" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="593" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A593" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="594" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A594" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="595" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A595" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="596" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A596" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="597" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A597" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="598" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A598" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="599" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A599" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="600" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A600" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="601" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A601" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="602" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A602" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="603" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A603" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="604" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A604" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="605" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A605" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="606" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A606" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="607" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A607" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="608" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A608" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="609" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A609" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="610" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A610" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="611" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A611" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="612" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A612" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="613" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A613" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="614" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A614" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="615" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A615" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="616" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A616" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="617" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A617" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="618" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A618" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="619" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A619" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="620" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A620" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="621" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A621" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="622" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A622" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="623" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A623" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="624" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A624" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="625" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A625" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="626" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A626" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="627" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A627" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="628" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A628" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="629" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A629" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="630" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A630" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="631" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A631" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="632" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A632" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="633" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A633" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="634" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A634" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="635" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A635" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="636" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A636" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="637" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A637" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="638" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A638" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="639" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A639" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="640" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A640" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="641" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A641" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="642" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A642" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="643" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A643" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="644" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A644" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="645" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A645" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="646" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A646" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="647" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A647" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="648" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A648" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="649" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A649" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="650" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A650" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="651" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A651" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="652" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A652" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="653" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A653" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="654" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A654" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="655" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A655" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="656" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A656" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="657" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A657" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="658" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A658" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="659" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A659" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="660" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A660" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="661" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A661" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="662" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A662" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="663" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A663" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="664" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A664" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="665" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A665" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="666" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A666" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="667" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A667" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="668" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A668" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="669" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A669" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="670" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A670" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="671" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A671" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="672" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A672" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="673" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A673" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="674" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A674" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="675" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A675" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="676" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A676" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="677" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A677" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="678" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A678" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="679" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A679" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="680" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A680" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="681" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A681" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="682" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A682" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="683" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A683" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="684" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A684" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="685" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A685" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="686" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A686" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="687" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A687" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="688" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A688" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="689" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A689" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="690" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A690" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="691" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A691" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="692" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A692" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="693" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A693" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="694" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A694" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="695" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A695" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="696" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A696" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="697" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A697" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="698" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A698" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="699" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A699" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="700" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A700" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="701" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A701" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="702" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A702" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="703" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A703" s="1" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="704" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A704" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="705" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A705" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="706" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A706" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="707" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A707" s="1" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="708" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A708" s="2" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="708" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A708" s="2" t="s">
+    <row r="709" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A709" s="2" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="709" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A709" s="2" t="s">
+    <row r="710" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A710" s="2" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="710" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A710" s="2" t="s">
+    <row r="711" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A711" s="2" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="711" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A711" s="2" t="s">
+    <row r="712" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A712" s="2" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="712" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A712" s="2" t="s">
+    <row r="713" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A713" s="2" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="713" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A713" s="2" t="s">
+    <row r="714" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A714" s="2" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="714" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A714" s="2" t="s">
+    <row r="715" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A715" s="2" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="715" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A715" s="2" t="s">
+    <row r="716" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A716" s="2" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="716" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A716" s="2" t="s">
+    <row r="717" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A717" s="2" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="717" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A717" s="2" t="s">
+    <row r="718" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A718" s="2" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="718" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A718" s="2" t="s">
+    <row r="719" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A719" s="2" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="719" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A719" s="2" t="s">
+    <row r="720" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A720" s="2" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="720" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A720" s="2" t="s">
+    <row r="721" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A721" s="2" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="721" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A721" s="2" t="s">
+    <row r="722" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A722" s="2" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="722" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A722" s="2" t="s">
+    <row r="723" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A723" s="2" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="723" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A723" s="2" t="s">
+    <row r="724" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A724" s="2" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="724" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A724" s="2" t="s">
+    <row r="725" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A725" s="2" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="725" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A725" s="2" t="s">
+    <row r="726" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A726" s="2" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="726" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A726" s="2" t="s">
+    <row r="727" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A727" s="2" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="727" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A727" s="2" t="s">
+    <row r="728" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A728" s="2" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="728" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A728" s="2" t="s">
+    <row r="729" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A729" s="2" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="729" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A729" s="2" t="s">
+    <row r="730" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A730" s="2" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="730" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A730" s="2" t="s">
+    <row r="731" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A731" s="2" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="731" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A731" s="2" t="s">
+    <row r="732" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A732" s="2" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="732" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A732" s="2" t="s">
+    <row r="733" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A733" s="2" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="733" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A733" s="2" t="s">
+    <row r="734" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A734" s="2" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="734" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A734" s="2" t="s">
+    <row r="735" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A735" s="2" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="735" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A735" s="2" t="s">
+    <row r="736" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A736" s="2" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="736" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A736" s="2" t="s">
+    <row r="737" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A737" s="2" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="737" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A737" s="2" t="s">
+    <row r="738" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A738" s="2" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="738" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A738" s="2" t="s">
+    <row r="739" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A739" s="2" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="739" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A739" s="2" t="s">
+    <row r="740" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A740" s="2" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="740" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A740" s="2" t="s">
+    <row r="741" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A741" s="2" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="741" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A741" s="2" t="s">
+    <row r="742" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A742" s="2" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="742" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A742" s="2" t="s">
+    <row r="743" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A743" s="2" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="743" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A743" s="2" t="s">
+    <row r="744" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A744" s="2" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="744" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A744" s="2" t="s">
+    <row r="745" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A745" s="2" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="745" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A745" s="2" t="s">
+    <row r="746" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A746" s="2" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="746" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A746" s="2" t="s">
+    <row r="747" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A747" s="2" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="747" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A747" s="2" t="s">
+    <row r="748" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A748" s="2" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="748" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A748" s="2" t="s">
+    <row r="749" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A749" s="2" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="749" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A749" s="2" t="s">
+    <row r="750" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A750" s="2" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="750" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A750" s="2" t="s">
+    <row r="751" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A751" s="2" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="751" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A751" s="2" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="752" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="752" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>